<commit_message>
Trying to fix error being thrown of generiateTableAndInsertStatement not defined
</commit_message>
<xml_diff>
--- a/python/test_py_bot.xlsx
+++ b/python/test_py_bot.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2977af2d0247e2aa/repos/todue/ToDue/python/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clazerone\Desktop\todue\ToDue\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3065BBC4-8868-4AC9-A602-0F2DB69ABCA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197D57C7-66B0-48F3-A520-8A55FBE61EDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4785" yWindow="1050" windowWidth="21600" windowHeight="11295" xr2:uid="{DD8FC68F-BA10-437D-A939-5DCB336219C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{929D5509-26D2-4384-8C75-DABE683C6389}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>hello</t>
+    <t>hi</t>
   </si>
   <si>
-    <t>hi</t>
+    <t>hello</t>
   </si>
 </sst>
 </file>
@@ -392,12 +392,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C901792D-8CEC-4D27-8A78-4F959E26DF7C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314C896C-0F88-4CD8-B23B-1C1162964EF9}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>